<commit_message>
conflicts of interest table
</commit_message>
<xml_diff>
--- a/data/PECO (23.10.19).xlsx
+++ b/data/PECO (23.10.19).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2286432b\OneDrive - University of Glasgow\R Studio - home folder\Citation network analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2286432b\OneDrive - University of Glasgow\R Studio - home folder\Citation network analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_217FB7D5F616E0E8EEA79592FEDA7BBBC1C41894" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2D54CBA1-D9A4-43DA-91B8-9374C37C9468}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_217FB7D5F616E0E8EEA79592FEDA7BBBC1C41894" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{014AC68E-94C7-4A9B-AA7B-F1D2299E9010}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PECO Full" sheetId="3" r:id="rId1"/>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2141,7 @@
         <v>8</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>375</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4179,9 +4179,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4317,26 +4320,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4360,9 +4352,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>